<commit_message>
[Rao] Commit for backup
</commit_message>
<xml_diff>
--- a/Design/Levels.xlsx
+++ b/Design/Levels.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="16600" activeTab="1"/>
+    <workbookView xWindow="9300" yWindow="460" windowWidth="24300" windowHeight="16600"/>
   </bookViews>
   <sheets>
-    <sheet name="_Design Points" sheetId="1" r:id="rId1"/>
-    <sheet name="_TASKS" sheetId="2" r:id="rId2"/>
+    <sheet name="BoardElements" sheetId="3" r:id="rId1"/>
+    <sheet name="_Design Points" sheetId="1" r:id="rId2"/>
+    <sheet name="_TASKS" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="91">
   <si>
     <t>Two decks of cards shuffle logic</t>
   </si>
@@ -194,6 +195,114 @@
   <si>
     <t>=====</t>
   </si>
+  <si>
+    <t>Splash &amp; Puzzle transitions</t>
+  </si>
+  <si>
+    <t>Scoring &amp; Result logic</t>
+  </si>
+  <si>
+    <t>ChipUI</t>
+  </si>
+  <si>
+    <t>UI animations</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>xIndex</t>
+  </si>
+  <si>
+    <t>yIndex</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>_notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CardType </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CT_TOTAL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CardColor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CC_TOTAL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CardNumber </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_5,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_7,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_9,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_J,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_K,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_TOTAL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CT_SPADE, (0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CC_RED, (0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_2, (0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_3, (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_4, (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_6, (4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_8, (6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_10, (8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_Q, (10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CN_A, (12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CT_CLUB,  (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CT_DIAMOND, (3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CT_HEART, (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    E_CC_BLACK, (1)</t>
+  </si>
 </sst>
 </file>
 
@@ -264,7 +373,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -274,6 +383,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -577,11 +689,1436 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="12980" ySplit="740" topLeftCell="I19" activePane="bottomLeft"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="6" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="10.83203125" style="7"/>
+    <col min="7" max="7" width="38" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="7">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F2" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>-1</v>
+      </c>
+      <c r="E11" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>0</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7">
+        <v>2</v>
+      </c>
+      <c r="F12" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>1</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7">
+        <v>2</v>
+      </c>
+      <c r="F13" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7">
+        <v>2</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>3</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7">
+        <v>2</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>4</v>
+      </c>
+      <c r="B16" s="7">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7">
+        <v>2</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>5</v>
+      </c>
+      <c r="B17" s="7">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>6</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>7</v>
+      </c>
+      <c r="B19" s="7">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>8</v>
+      </c>
+      <c r="B20" s="7">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>9</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>0</v>
+      </c>
+      <c r="B22" s="7">
+        <v>2</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7">
+        <v>2</v>
+      </c>
+      <c r="F22" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>1</v>
+      </c>
+      <c r="B23" s="7">
+        <v>2</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2</v>
+      </c>
+      <c r="D23" s="7">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>2</v>
+      </c>
+      <c r="B24" s="7">
+        <v>2</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0</v>
+      </c>
+      <c r="E24" s="7">
+        <v>3</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>3</v>
+      </c>
+      <c r="B25" s="7">
+        <v>2</v>
+      </c>
+      <c r="C25" s="7">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0</v>
+      </c>
+      <c r="E25" s="7">
+        <v>3</v>
+      </c>
+      <c r="F25" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>4</v>
+      </c>
+      <c r="B26" s="7">
+        <v>2</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0</v>
+      </c>
+      <c r="E26" s="7">
+        <v>3</v>
+      </c>
+      <c r="F26" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>5</v>
+      </c>
+      <c r="B27" s="7">
+        <v>2</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0</v>
+      </c>
+      <c r="E27" s="7">
+        <v>3</v>
+      </c>
+      <c r="F27" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>6</v>
+      </c>
+      <c r="B28" s="7">
+        <v>2</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0</v>
+      </c>
+      <c r="E28" s="7">
+        <v>3</v>
+      </c>
+      <c r="F28" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
+        <v>7</v>
+      </c>
+      <c r="B29" s="7">
+        <v>2</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1</v>
+      </c>
+      <c r="D29" s="7">
+        <v>0</v>
+      </c>
+      <c r="E29" s="7">
+        <v>3</v>
+      </c>
+      <c r="F29" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
+        <v>8</v>
+      </c>
+      <c r="B30" s="7">
+        <v>2</v>
+      </c>
+      <c r="C30" s="7">
+        <v>1</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0</v>
+      </c>
+      <c r="E30" s="7">
+        <v>1</v>
+      </c>
+      <c r="F30" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
+        <v>9</v>
+      </c>
+      <c r="B31" s="7">
+        <v>2</v>
+      </c>
+      <c r="C31" s="7">
+        <v>1</v>
+      </c>
+      <c r="D31" s="7">
+        <v>1</v>
+      </c>
+      <c r="E31" s="7">
+        <v>0</v>
+      </c>
+      <c r="F31" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>0</v>
+      </c>
+      <c r="B32" s="7">
+        <v>3</v>
+      </c>
+      <c r="C32" s="7">
+        <v>1</v>
+      </c>
+      <c r="D32" s="7">
+        <v>1</v>
+      </c>
+      <c r="E32" s="7">
+        <v>2</v>
+      </c>
+      <c r="F32" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
+        <v>1</v>
+      </c>
+      <c r="B33" s="7">
+        <v>3</v>
+      </c>
+      <c r="C33" s="7">
+        <v>2</v>
+      </c>
+      <c r="D33" s="7">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0</v>
+      </c>
+      <c r="F33" s="7">
+        <v>10</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
+        <v>2</v>
+      </c>
+      <c r="B34" s="7">
+        <v>3</v>
+      </c>
+      <c r="C34" s="7">
+        <v>2</v>
+      </c>
+      <c r="D34" s="7">
+        <v>1</v>
+      </c>
+      <c r="E34" s="7">
+        <v>2</v>
+      </c>
+      <c r="F34" s="7">
+        <v>4</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
+        <v>3</v>
+      </c>
+      <c r="B35" s="7">
+        <v>3</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2</v>
+      </c>
+      <c r="D35" s="7">
+        <v>1</v>
+      </c>
+      <c r="E35" s="7">
+        <v>2</v>
+      </c>
+      <c r="F35" s="7">
+        <v>3</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
+        <v>4</v>
+      </c>
+      <c r="B36" s="7">
+        <v>3</v>
+      </c>
+      <c r="C36" s="7">
+        <v>2</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1</v>
+      </c>
+      <c r="E36" s="7">
+        <v>2</v>
+      </c>
+      <c r="F36" s="7">
+        <v>2</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="7">
+        <v>5</v>
+      </c>
+      <c r="B37" s="7">
+        <v>3</v>
+      </c>
+      <c r="C37" s="7">
+        <v>2</v>
+      </c>
+      <c r="D37" s="7">
+        <v>1</v>
+      </c>
+      <c r="E37" s="7">
+        <v>2</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="7">
+        <v>6</v>
+      </c>
+      <c r="B38" s="7">
+        <v>3</v>
+      </c>
+      <c r="C38" s="7">
+        <v>2</v>
+      </c>
+      <c r="D38" s="7">
+        <v>1</v>
+      </c>
+      <c r="E38" s="7">
+        <v>2</v>
+      </c>
+      <c r="F38" s="7">
+        <v>0</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
+        <v>7</v>
+      </c>
+      <c r="B39" s="7">
+        <v>3</v>
+      </c>
+      <c r="C39" s="7">
+        <v>1</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0</v>
+      </c>
+      <c r="E39" s="7">
+        <v>3</v>
+      </c>
+      <c r="F39" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="7">
+        <v>8</v>
+      </c>
+      <c r="B40" s="7">
+        <v>3</v>
+      </c>
+      <c r="C40" s="7">
+        <v>1</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0</v>
+      </c>
+      <c r="E40" s="7">
+        <v>1</v>
+      </c>
+      <c r="F40" s="7">
+        <v>6</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="7">
+        <v>9</v>
+      </c>
+      <c r="B41" s="7">
+        <v>3</v>
+      </c>
+      <c r="C41" s="7">
+        <v>1</v>
+      </c>
+      <c r="D41" s="7">
+        <v>1</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0</v>
+      </c>
+      <c r="F41" s="7">
+        <v>10</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="7">
+        <v>0</v>
+      </c>
+      <c r="B42" s="7">
+        <v>4</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="7">
+        <v>1</v>
+      </c>
+      <c r="B43" s="7">
+        <v>4</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="7">
+        <v>2</v>
+      </c>
+      <c r="B44" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="7">
+        <v>3</v>
+      </c>
+      <c r="B45" s="7">
+        <v>4</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="7">
+        <v>4</v>
+      </c>
+      <c r="B46" s="7">
+        <v>4</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="7">
+        <v>5</v>
+      </c>
+      <c r="B47" s="7">
+        <v>4</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="7">
+        <v>6</v>
+      </c>
+      <c r="B48" s="7">
+        <v>4</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="7">
+        <v>7</v>
+      </c>
+      <c r="B49" s="7">
+        <v>4</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="7">
+        <v>8</v>
+      </c>
+      <c r="B50" s="7">
+        <v>4</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="7">
+        <v>9</v>
+      </c>
+      <c r="B51" s="7">
+        <v>4</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="7">
+        <v>0</v>
+      </c>
+      <c r="B52" s="7">
+        <v>5</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="7">
+        <v>1</v>
+      </c>
+      <c r="B53" s="7">
+        <v>5</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="7">
+        <v>2</v>
+      </c>
+      <c r="B54" s="7">
+        <v>5</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="7">
+        <v>3</v>
+      </c>
+      <c r="B55" s="7">
+        <v>5</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="7">
+        <v>4</v>
+      </c>
+      <c r="B56" s="7">
+        <v>5</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="7">
+        <v>5</v>
+      </c>
+      <c r="B57" s="7">
+        <v>5</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="7">
+        <v>6</v>
+      </c>
+      <c r="B58" s="7">
+        <v>5</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="7">
+        <v>7</v>
+      </c>
+      <c r="B59" s="7">
+        <v>5</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="7">
+        <v>8</v>
+      </c>
+      <c r="B60" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="7">
+        <v>9</v>
+      </c>
+      <c r="B61" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="7">
+        <v>0</v>
+      </c>
+      <c r="B62" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="7">
+        <v>1</v>
+      </c>
+      <c r="B63" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="7">
+        <v>2</v>
+      </c>
+      <c r="B64" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="7">
+        <v>3</v>
+      </c>
+      <c r="B65" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="7">
+        <v>4</v>
+      </c>
+      <c r="B66" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="7">
+        <v>5</v>
+      </c>
+      <c r="B67" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="7">
+        <v>6</v>
+      </c>
+      <c r="B68" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="7">
+        <v>7</v>
+      </c>
+      <c r="B69" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="7">
+        <v>8</v>
+      </c>
+      <c r="B70" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="7">
+        <v>9</v>
+      </c>
+      <c r="B71" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="7">
+        <v>0</v>
+      </c>
+      <c r="B72" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="7">
+        <v>1</v>
+      </c>
+      <c r="B73" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="7">
+        <v>2</v>
+      </c>
+      <c r="B74" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="7">
+        <v>3</v>
+      </c>
+      <c r="B75" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="7">
+        <v>4</v>
+      </c>
+      <c r="B76" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="7">
+        <v>5</v>
+      </c>
+      <c r="B77" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="7">
+        <v>6</v>
+      </c>
+      <c r="B78" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="7">
+        <v>7</v>
+      </c>
+      <c r="B79" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="7">
+        <v>8</v>
+      </c>
+      <c r="B80" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="7">
+        <v>9</v>
+      </c>
+      <c r="B81" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="7">
+        <v>0</v>
+      </c>
+      <c r="B82" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="7">
+        <v>1</v>
+      </c>
+      <c r="B83" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="7">
+        <v>2</v>
+      </c>
+      <c r="B84" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="7">
+        <v>3</v>
+      </c>
+      <c r="B85" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="7">
+        <v>4</v>
+      </c>
+      <c r="B86" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="7">
+        <v>5</v>
+      </c>
+      <c r="B87" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="7">
+        <v>6</v>
+      </c>
+      <c r="B88" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="7">
+        <v>7</v>
+      </c>
+      <c r="B89" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="7">
+        <v>8</v>
+      </c>
+      <c r="B90" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="7">
+        <v>9</v>
+      </c>
+      <c r="B91" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="7">
+        <v>0</v>
+      </c>
+      <c r="B92" s="7">
+        <v>9</v>
+      </c>
+      <c r="C92" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D92" s="7">
+        <v>-1</v>
+      </c>
+      <c r="E92" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F92" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="7">
+        <v>1</v>
+      </c>
+      <c r="B93" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="7">
+        <v>2</v>
+      </c>
+      <c r="B94" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="7">
+        <v>3</v>
+      </c>
+      <c r="B95" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="7">
+        <v>4</v>
+      </c>
+      <c r="B96" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="7">
+        <v>5</v>
+      </c>
+      <c r="B97" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="7">
+        <v>6</v>
+      </c>
+      <c r="B98" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="7">
+        <v>7</v>
+      </c>
+      <c r="B99" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="7">
+        <v>8</v>
+      </c>
+      <c r="B100" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="7">
+        <v>9</v>
+      </c>
+      <c r="B101" s="7">
+        <v>9</v>
+      </c>
+      <c r="C101" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D101" s="7">
+        <v>-1</v>
+      </c>
+      <c r="E101" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F101" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L30"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28592,27 +30129,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A2:M31"/>
+  <dimension ref="A2:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="4.1640625" customWidth="1"/>
-    <col min="8" max="8" width="1.83203125" customWidth="1"/>
-    <col min="9" max="9" width="16.5" customWidth="1"/>
-    <col min="10" max="10" width="3.1640625" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.5" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" customWidth="1"/>
+    <col min="15" max="15" width="16.5" customWidth="1"/>
+    <col min="16" max="16" width="3.1640625" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.5" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -28620,7 +30157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -28628,341 +30165,365 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" t="s">
+      <c r="O6" t="s">
         <v>53</v>
       </c>
-      <c r="K6" t="s">
+      <c r="Q6" t="s">
         <v>13</v>
       </c>
-      <c r="M6" t="s">
+      <c r="S6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="O7" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="K7" t="s">
+      <c r="Q7" t="s">
         <v>14</v>
       </c>
-      <c r="M7" t="s">
+      <c r="S7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H8" s="2"/>
-      <c r="I8" t="s">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="4">
+      <c r="P8" s="4">
         <v>1</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="Q8" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I9" t="s">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O9" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="4">
+      <c r="P9" s="4">
         <v>2</v>
       </c>
-      <c r="K9" t="s">
+      <c r="Q9" t="s">
         <v>15</v>
       </c>
-      <c r="M9" t="s">
+      <c r="S9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I10" s="2" t="s">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="4">
+      <c r="P10" s="4">
         <v>3</v>
       </c>
-      <c r="K10" t="s">
+      <c r="Q10" t="s">
         <v>16</v>
       </c>
-      <c r="M10" t="s">
+      <c r="S10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="4">
+      <c r="P11" s="4">
         <v>4</v>
       </c>
-      <c r="K11" s="6" t="s">
+      <c r="Q11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" t="s">
+      <c r="R11" s="3"/>
+      <c r="S11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H12" s="2"/>
-      <c r="I12" s="2" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="N12" s="2"/>
+      <c r="O12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="4">
+      <c r="P12" s="4">
         <v>5</v>
       </c>
-      <c r="K12" t="s">
+      <c r="Q12" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" t="s">
+      <c r="R12" s="3"/>
+      <c r="S12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="I13" t="s">
+      <c r="O13" t="s">
         <v>32</v>
       </c>
-      <c r="J13" s="4">
+      <c r="P13" s="4">
         <v>6</v>
       </c>
-      <c r="K13" t="s">
+      <c r="Q13" t="s">
         <v>19</v>
       </c>
-      <c r="M13" t="s">
+      <c r="S13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="4">
+      <c r="P14" s="4">
         <v>7</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="Q14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M14" t="s">
+      <c r="S14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="J15" s="4">
+      <c r="N15" s="2"/>
+      <c r="P15" s="4">
         <v>8</v>
       </c>
-      <c r="K15" t="s">
+      <c r="Q15" t="s">
         <v>21</v>
       </c>
-      <c r="M15" t="s">
+      <c r="S15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="4">
+      <c r="P16" s="4">
         <v>9</v>
       </c>
-      <c r="K16" t="s">
+      <c r="Q16" t="s">
         <v>22</v>
       </c>
-      <c r="M16" t="s">
+      <c r="S16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="4">
+      <c r="P17" s="4">
         <v>10</v>
       </c>
-      <c r="K17" t="s">
+      <c r="Q17" t="s">
         <v>23</v>
       </c>
-      <c r="M17" t="s">
+      <c r="S17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="I18" s="2" t="s">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="O18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J18" s="4">
+      <c r="P18" s="4">
         <v>11</v>
       </c>
-      <c r="K18" t="s">
+      <c r="Q18" t="s">
         <v>24</v>
       </c>
-      <c r="M18" t="s">
+      <c r="S18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="I19" s="2" t="s">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="O19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="4">
+      <c r="P19" s="4">
         <v>12</v>
       </c>
-      <c r="K19" t="s">
+      <c r="Q19" t="s">
         <v>25</v>
       </c>
-      <c r="M19" t="s">
+      <c r="S19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="I20" s="2" t="s">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="O20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J20" s="4">
+      <c r="P20" s="4">
         <v>13</v>
       </c>
-      <c r="K20" t="s">
+      <c r="Q20" t="s">
         <v>26</v>
       </c>
-      <c r="M20" t="s">
+      <c r="S20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="I21" s="2" t="s">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="O21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="4">
+      <c r="P21" s="4">
         <v>14</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="Q21" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>8</v>
       </c>
-      <c r="J22" s="4">
+      <c r="P22" s="4">
         <v>15</v>
       </c>
-      <c r="K22" t="s">
+      <c r="Q22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="I23" t="s">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="O23" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="4">
+      <c r="P23" s="4">
         <v>16</v>
       </c>
-      <c r="K23" t="s">
+      <c r="Q23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="I24" t="s">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="O24" t="s">
         <v>36</v>
       </c>
-      <c r="J24" s="4">
+      <c r="P24" s="4">
         <v>17</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="Q24" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="I25" t="s">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="O25" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="4">
+      <c r="P25" s="4">
         <v>18</v>
       </c>
-      <c r="K25" t="s">
+      <c r="Q25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="J26" s="4">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="P26" s="4">
         <v>19</v>
       </c>
-      <c r="K26" t="s">
+      <c r="Q26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="J27" s="4">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="P27" s="4">
         <v>20</v>
       </c>
-      <c r="K27" t="s">
+      <c r="Q27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="J28" s="4">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="P28" s="4">
         <v>21</v>
       </c>
-      <c r="K28" s="6" t="s">
+      <c r="Q28" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="J29" s="4">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="P29" s="4">
         <v>22</v>
       </c>
-      <c r="K29" s="6" t="s">
+      <c r="Q29" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="J30" s="4">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="P30" s="4">
         <v>23</v>
       </c>
-      <c r="K30" t="s">
+      <c r="Q30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="J31" s="4">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="P31" s="4">
         <v>24</v>
       </c>
-      <c r="K31" s="6" t="s">
+      <c r="Q31" s="6" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>